<commit_message>
modify: integration for noLique in calcLiquefaction
</commit_message>
<xml_diff>
--- a/test-doc/液化/各方法結果比較(貼入mat).xlsx
+++ b/test-doc/液化/各方法結果比較(貼入mat).xlsx
@@ -1,28 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20375"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20379"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\開源-JS-003-2-w-geo\w-geo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\開源-JS-003-2-w-geo\w-geo\test-doc\液化\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CFA131C-FC90-4381-BAE9-32B6CAFE0C1C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A14890DA-FEF9-4B61-95DA-74FAA1F07CDC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9144" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="mat" sheetId="1" r:id="rId1"/>
     <sheet name="各方法FS比較" sheetId="2" r:id="rId2"/>
-    <sheet name="各方法結果比較" sheetId="3" r:id="rId3"/>
+    <sheet name="各方法PL比較" sheetId="4" r:id="rId3"/>
+    <sheet name="各方法結果比較" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="954" uniqueCount="207">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="954" uniqueCount="206">
   <si>
     <t>depthStart</t>
   </si>
@@ -498,9 +499,6 @@
     <t>-</t>
   </si>
   <si>
-    <t>D50 非數字，略過部份非液化條件檢核, D10 非數字，略過部份非液化條件檢核</t>
-  </si>
-  <si>
     <t>3.525</t>
   </si>
   <si>
@@ -528,18 +526,6 @@
     <t>14</t>
   </si>
   <si>
-    <t>Volumetric Strain(Tokimatsu And Seed): 出現外插情形 N160=38.29626079871692 &gt; N160Max=33.845439845659584，依照CSR=0.4145107783481977並給予最小體積應變vstr=0.1%, Volumetric Strain(Ishihara And Yoshimine): 出現外插情形 N172=31.913550665597437 &gt; N172Max=30，依照FS=2並給予最小體積應變vstr=0%</t>
-  </si>
-  <si>
-    <t>PI 非數字與非NP，略過部份非液化條件檢核</t>
-  </si>
-  <si>
-    <t>D50 非數字，略過部份非液化條件檢核, D10 非數字，略過部份非液化條件檢核, vibrationType 非數字, vibrationType[0] 不等於 1 或 2，更改為預設值1, Volumetric Strain(Tokimatsu And Seed): CSR大於0.6超過原研究範疇，強制改為0.6, Volumetric Strain(Tokimatsu And Seed): 出現外插情形 N160=37.150772494769974 &gt; N160Max=36.7，依照CSR=0.6並給予最小體積應變vstr=0.1%, Volumetric Strain(Ishihara And Yoshimine): 出現外插情形 N172=30.958977078974982 &gt; N172Max=30，依照FS=2並給予最小體積應變vstr=0%</t>
-  </si>
-  <si>
-    <t>Volumetric Strain(Tokimatsu And Seed): 出現外插情形 N160=37.150772494769974 &gt; N160Max=33.348948148804865，依照CSR=0.3996625660206793並給予最小體積應變vstr=0.1%, Volumetric Strain(Ishihara And Yoshimine): 出現外插情形 N172=30.958977078974982 &gt; N172Max=30，依照FS=2並給予最小體積應變vstr=0%</t>
-  </si>
-  <si>
     <t>6.525</t>
   </si>
   <si>
@@ -549,15 +535,6 @@
     <t>12</t>
   </si>
   <si>
-    <t>Volumetric Strain(Tokimatsu And Seed): 出現外插情形 N160=38.07293279469695 &gt; N160Max=33.752136934605055，依照CSR=0.4117850004466762並給予最小體積應變vstr=0.1%, Volumetric Strain(Ishihara And Yoshimine): 出現外插情形 N172=31.727443995580796 &gt; N172Max=30，依照FS=2並給予最小體積應變vstr=0%</t>
-  </si>
-  <si>
-    <t>D50 非數字，略過部份非液化條件檢核, D10 非數字，略過部份非液化條件檢核, vibrationType 非數字, vibrationType[0] 不等於 1 或 2，更改為預設值1, Volumetric Strain(Tokimatsu And Seed): CSR大於0.6超過原研究範疇，強制改為0.6, Volumetric Strain(Tokimatsu And Seed): 出現外插情形 N160=38.05808075175254 &gt; N160Max=36.7，依照CSR=0.6並給予最小體積應變vstr=0.1%, Volumetric Strain(Ishihara And Yoshimine): 出現外插情形 N172=31.715067293127117 &gt; N172Max=30，依照FS=2並給予最小體積應變vstr=0%</t>
-  </si>
-  <si>
-    <t>Volumetric Strain(Tokimatsu And Seed): 出現外插情形 N160=38.05808075175254 &gt; N160Max=33.10466537238953，依照CSR=0.3919704067448309並給予最小體積應變vstr=0.1%, Volumetric Strain(Ishihara And Yoshimine): 出現外插情形 N172=31.715067293127117 &gt; N172Max=30，依照FS=2並給予最小體積應變vstr=0%</t>
-  </si>
-  <si>
     <t>8.025</t>
   </si>
   <si>
@@ -567,9 +544,6 @@
     <t>15</t>
   </si>
   <si>
-    <t>D50 非數字，略過部份非液化條件檢核, D10 非數字，略過部份非液化條件檢核, vibrationType 非數字, vibrationType[0] 不等於 1 或 2，更改為預設值1</t>
-  </si>
-  <si>
     <t>9.525</t>
   </si>
   <si>
@@ -618,9 +592,6 @@
     <t>出現外插情形 FC=45 &gt; FCMax=35，依據最近2點外插CRR75=0.1799596328461885</t>
   </si>
   <si>
-    <t>D50 非數字，略過部份非液化條件檢核, D10 非數字，略過部份非液化條件檢核, PI 非數字與非NP，略過部份非液化條件檢核, vibrationType 非數字, vibrationType[0] 不等於 1 或 2，更改為預設值1</t>
-  </si>
-  <si>
     <t>17.025</t>
   </si>
   <si>
@@ -642,14 +613,41 @@
     <t>94</t>
   </si>
   <si>
-    <t>D50 非數字，略過部份非液化條件檢核, D10 非數字，略過部份非液化條件檢核, vibrationType 非數字, vibrationType[0] 不等於 1 或 2，更改為預設值1, Volumetric Strain(Tokimatsu And Seed): CSR大於0.6超過原研究範疇，強制改為0.6</t>
+    <t>PI非數字與非NP，強制略過部份非液化條件檢核</t>
+  </si>
+  <si>
+    <t>D50非數字，強制略過部份非液化條件檢核; D10非數字，強制略過部份非液化條件檢核; vibrationType非數字; Volumetric Strain(Tokimatsu And Seed): CSR大於0.6超過原研究範疇，強制改為0.6</t>
+  </si>
+  <si>
+    <t>CRR75[18.765665696998305]大於0.6超過原研究範疇，強制改為0.6; Volumetric Strain(Tokimatsu And Seed): 出現外插情形 N160=38.29626079871692 &gt; N160Max=33.845439845659584，依照CSR=0.4145107783481977並給予最小體積應變vstr=0.1%; Volumetric Strain(Ishihara And Yoshimine): 出現外插情形 N172=31.913550665597437 &gt; N172Max=30，依照FS=1.447489501698765並給予最小體積應變vstr=0.11307814700732616%</t>
+  </si>
+  <si>
+    <t>D50非數字，強制略過部份非液化條件檢核; D10非數字，強制略過部份非液化條件檢核; vibrationType非數字; Volumetric Strain(Tokimatsu And Seed): CSR大於0.6超過原研究範疇，強制改為0.6; Volumetric Strain(Tokimatsu And Seed): 出現外插情形 N160=37.150772494769974 &gt; N160Max=36.7，依照CSR=0.6並給予最小體積應變vstr=0.1%; Volumetric Strain(Ishihara And Yoshimine): 出現外插情形 N172=30.958977078974982 &gt; N172Max=30，依照FS=2並給予最小體積應變vstr=0%</t>
+  </si>
+  <si>
+    <t>Volumetric Strain(Tokimatsu And Seed): 出現外插情形 N160=37.150772494769974 &gt; N160Max=33.348948148804865，依照CSR=0.3996625660206793並給予最小體積應變vstr=0.1%; Volumetric Strain(Ishihara And Yoshimine): 出現外插情形 N172=30.958977078974982 &gt; N172Max=30，依照FS=2並給予最小體積應變vstr=0%</t>
+  </si>
+  <si>
+    <t>CRR75[17.23857654291693]大於0.6超過原研究範疇，強制改為0.6; Volumetric Strain(Tokimatsu And Seed): 出現外插情形 N160=38.07293279469695 &gt; N160Max=33.752136934605055，依照CSR=0.4117850004466762並給予最小體積應變vstr=0.1%; Volumetric Strain(Ishihara And Yoshimine): 出現外插情形 N172=31.727443995580796 &gt; N172Max=30，依照FS=1.4570710427751399並給予最小體積應變vstr=0.11003867064062244%</t>
+  </si>
+  <si>
+    <t>D50非數字，強制略過部份非液化條件檢核; D10非數字，強制略過部份非液化條件檢核; vibrationType非數字; Volumetric Strain(Tokimatsu And Seed): CSR大於0.6超過原研究範疇，強制改為0.6; Volumetric Strain(Tokimatsu And Seed): 出現外插情形 N160=38.05808075175254 &gt; N160Max=36.7，依照CSR=0.6並給予最小體積應變vstr=0.1%; Volumetric Strain(Ishihara And Yoshimine): 出現外插情形 N172=31.715067293127117 &gt; N172Max=30，依照FS=2並給予最小體積應變vstr=0%</t>
+  </si>
+  <si>
+    <t>Volumetric Strain(Tokimatsu And Seed): 出現外插情形 N160=38.05808075175254 &gt; N160Max=33.10466537238953，依照CSR=0.3919704067448309並給予最小體積應變vstr=0.1%; Volumetric Strain(Ishihara And Yoshimine): 出現外插情形 N172=31.715067293127117 &gt; N172Max=30，依照FS=2並給予最小體積應變vstr=0%</t>
+  </si>
+  <si>
+    <t>D50非數字，強制略過部份非液化條件檢核; D10非數字，強制略過部份非液化條件檢核; vibrationType非數字</t>
+  </si>
+  <si>
+    <t>PI非數字與非NP，強制略過部份非液化條件檢核; D50非數字，強制略過部份非液化條件檢核; D10非數字，強制略過部份非液化條件檢核; vibrationType非數字</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -674,6 +672,19 @@
     <font>
       <sz val="10"/>
       <color rgb="FFFF0000"/>
+      <name val="微軟正黑體"/>
+      <family val="2"/>
+      <charset val="136"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="微軟正黑體"/>
+      <family val="2"/>
+      <charset val="136"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="0" tint="-0.14999847407452621"/>
       <name val="微軟正黑體"/>
       <family val="2"/>
       <charset val="136"/>
@@ -705,11 +716,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="一般" xfId="0" builtinId="0"/>
@@ -1051,8 +1064,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:EQ14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView topLeftCell="AE1" workbookViewId="0">
+      <selection activeCell="AS1" sqref="AS1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.2" x14ac:dyDescent="0.3"/>
@@ -1838,7 +1851,7 @@
         <v>0</v>
       </c>
       <c r="DI2" t="s">
-        <v>206</v>
+        <v>197</v>
       </c>
       <c r="DJ2">
         <v>0.98481249999999998</v>
@@ -1895,7 +1908,7 @@
         <v>0</v>
       </c>
       <c r="EB2" t="s">
-        <v>206</v>
+        <v>197</v>
       </c>
       <c r="EC2">
         <v>0.98481249999999998</v>
@@ -1948,7 +1961,7 @@
         <v>148</v>
       </c>
       <c r="B3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C3">
         <v>2.7749999999999999</v>
@@ -1969,25 +1982,25 @@
         <v>149</v>
       </c>
       <c r="I3" t="s">
+        <v>159</v>
+      </c>
+      <c r="J3" t="s">
         <v>160</v>
       </c>
-      <c r="J3" t="s">
+      <c r="K3" t="s">
+        <v>149</v>
+      </c>
+      <c r="L3" t="s">
+        <v>149</v>
+      </c>
+      <c r="M3" t="s">
+        <v>149</v>
+      </c>
+      <c r="N3" t="s">
+        <v>149</v>
+      </c>
+      <c r="O3" t="s">
         <v>161</v>
-      </c>
-      <c r="K3" t="s">
-        <v>149</v>
-      </c>
-      <c r="L3" t="s">
-        <v>149</v>
-      </c>
-      <c r="M3" t="s">
-        <v>149</v>
-      </c>
-      <c r="N3" t="s">
-        <v>149</v>
-      </c>
-      <c r="O3" t="s">
-        <v>162</v>
       </c>
       <c r="P3" t="s">
         <v>149</v>
@@ -2014,7 +2027,7 @@
         <v>149</v>
       </c>
       <c r="X3" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="Y3" t="s">
         <v>149</v>
@@ -2281,7 +2294,7 @@
         <v>0</v>
       </c>
       <c r="DI3" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
       <c r="DJ3" t="s">
         <v>149</v>
@@ -2338,7 +2351,7 @@
         <v>0</v>
       </c>
       <c r="EB3" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
       <c r="EC3" t="s">
         <v>149</v>
@@ -2388,10 +2401,10 @@
     </row>
     <row r="4" spans="1:147" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B4" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C4">
         <v>4.2750000000000004</v>
@@ -2412,25 +2425,25 @@
         <v>149</v>
       </c>
       <c r="I4" t="s">
+        <v>164</v>
+      </c>
+      <c r="J4" t="s">
         <v>165</v>
       </c>
-      <c r="J4" t="s">
+      <c r="K4" t="s">
+        <v>149</v>
+      </c>
+      <c r="L4" t="s">
+        <v>149</v>
+      </c>
+      <c r="M4" t="s">
+        <v>149</v>
+      </c>
+      <c r="N4" t="s">
+        <v>149</v>
+      </c>
+      <c r="O4" t="s">
         <v>166</v>
-      </c>
-      <c r="K4" t="s">
-        <v>149</v>
-      </c>
-      <c r="L4" t="s">
-        <v>149</v>
-      </c>
-      <c r="M4" t="s">
-        <v>149</v>
-      </c>
-      <c r="N4" t="s">
-        <v>149</v>
-      </c>
-      <c r="O4" t="s">
-        <v>167</v>
       </c>
       <c r="P4" t="s">
         <v>149</v>
@@ -2508,16 +2521,16 @@
         <v>0.41451077834819772</v>
       </c>
       <c r="AO4">
-        <v>18.765665696998305</v>
+        <v>0.6</v>
       </c>
       <c r="AP4">
-        <v>10</v>
+        <v>1.447489501698765</v>
       </c>
       <c r="AQ4">
         <v>0.1</v>
       </c>
       <c r="AR4">
-        <v>0</v>
+        <v>0.11307814700732616</v>
       </c>
       <c r="AS4">
         <v>1.3177443014899113</v>
@@ -2526,10 +2539,10 @@
         <v>3.8630504301387543E-2</v>
       </c>
       <c r="AU4">
-        <v>3.4896234280900613E-2</v>
+        <v>3.6592406486010504E-2</v>
       </c>
       <c r="AV4" t="s">
-        <v>168</v>
+        <v>198</v>
       </c>
       <c r="AW4">
         <v>0.95725000000000005</v>
@@ -2574,7 +2587,7 @@
         <v>4.9720196549436158E-2</v>
       </c>
       <c r="BK4" t="s">
-        <v>169</v>
+        <v>149</v>
       </c>
       <c r="BL4">
         <v>0.95725000000000005</v>
@@ -2619,7 +2632,7 @@
         <v>4.9720196549436158E-2</v>
       </c>
       <c r="BZ4" t="s">
-        <v>169</v>
+        <v>149</v>
       </c>
       <c r="CA4">
         <v>0.9706445078134921</v>
@@ -2724,7 +2737,7 @@
         <v>0</v>
       </c>
       <c r="DI4" t="s">
-        <v>170</v>
+        <v>199</v>
       </c>
       <c r="DJ4">
         <v>0.93587500000000001</v>
@@ -2781,7 +2794,7 @@
         <v>0</v>
       </c>
       <c r="EB4" t="s">
-        <v>170</v>
+        <v>199</v>
       </c>
       <c r="EC4">
         <v>0.93587500000000001</v>
@@ -2826,15 +2839,15 @@
         <v>5.4434985275812371E-3</v>
       </c>
       <c r="EQ4" t="s">
-        <v>171</v>
+        <v>200</v>
       </c>
     </row>
     <row r="5" spans="1:147" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B5" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="C5">
         <v>5.7750000000000004</v>
@@ -2855,10 +2868,10 @@
         <v>149</v>
       </c>
       <c r="I5" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="J5" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="K5" t="s">
         <v>149</v>
@@ -2873,7 +2886,7 @@
         <v>149</v>
       </c>
       <c r="O5" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="P5" t="s">
         <v>149</v>
@@ -2951,16 +2964,16 @@
         <v>0.41178500044667621</v>
       </c>
       <c r="AO5">
-        <v>17.238576542916931</v>
+        <v>0.6</v>
       </c>
       <c r="AP5">
-        <v>10</v>
+        <v>1.4570710427751399</v>
       </c>
       <c r="AQ5">
         <v>0.1</v>
       </c>
       <c r="AR5">
-        <v>0</v>
+        <v>0.11003867064062244</v>
       </c>
       <c r="AS5">
         <v>1.3177443014899113</v>
@@ -2969,10 +2982,10 @@
         <v>4.0130504301387544E-2</v>
       </c>
       <c r="AU5">
-        <v>3.4896234280900613E-2</v>
+        <v>3.8242986545619841E-2</v>
       </c>
       <c r="AV5" t="s">
-        <v>175</v>
+        <v>201</v>
       </c>
       <c r="AW5">
         <v>0.94225000000000003</v>
@@ -3017,7 +3030,7 @@
         <v>4.9720196549436158E-2</v>
       </c>
       <c r="BK5" t="s">
-        <v>169</v>
+        <v>149</v>
       </c>
       <c r="BL5">
         <v>0.94225000000000003</v>
@@ -3062,7 +3075,7 @@
         <v>4.9720196549436158E-2</v>
       </c>
       <c r="BZ5" t="s">
-        <v>169</v>
+        <v>149</v>
       </c>
       <c r="CA5">
         <v>0.95954724721815465</v>
@@ -3167,7 +3180,7 @@
         <v>0</v>
       </c>
       <c r="DI5" t="s">
-        <v>176</v>
+        <v>202</v>
       </c>
       <c r="DJ5">
         <v>0.91337500000000005</v>
@@ -3224,7 +3237,7 @@
         <v>0</v>
       </c>
       <c r="EB5" t="s">
-        <v>176</v>
+        <v>202</v>
       </c>
       <c r="EC5">
         <v>0.91337500000000005</v>
@@ -3269,15 +3282,15 @@
         <v>5.4434985275812371E-3</v>
       </c>
       <c r="EQ5" t="s">
-        <v>177</v>
+        <v>203</v>
       </c>
     </row>
     <row r="6" spans="1:147" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="B6" t="s">
-        <v>178</v>
+        <v>170</v>
       </c>
       <c r="C6">
         <v>7.2750000000000004</v>
@@ -3298,10 +3311,10 @@
         <v>149</v>
       </c>
       <c r="I6" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="J6" t="s">
-        <v>179</v>
+        <v>171</v>
       </c>
       <c r="K6" t="s">
         <v>149</v>
@@ -3316,7 +3329,7 @@
         <v>149</v>
       </c>
       <c r="O6" t="s">
-        <v>180</v>
+        <v>172</v>
       </c>
       <c r="P6" t="s">
         <v>149</v>
@@ -3412,7 +3425,7 @@
         <v>5.9313241528055206E-2</v>
       </c>
       <c r="AU6">
-        <v>4.4079123330625233E-2</v>
+        <v>4.7425875595344461E-2</v>
       </c>
       <c r="AV6" t="s">
         <v>149</v>
@@ -3460,7 +3473,7 @@
         <v>6.2337632172385492E-2</v>
       </c>
       <c r="BK6" t="s">
-        <v>169</v>
+        <v>196</v>
       </c>
       <c r="BL6">
         <v>0.92725000000000002</v>
@@ -3505,7 +3518,7 @@
         <v>6.2337632172385492E-2</v>
       </c>
       <c r="BZ6" t="s">
-        <v>169</v>
+        <v>196</v>
       </c>
       <c r="CA6">
         <v>0.94568291693141515</v>
@@ -3610,7 +3623,7 @@
         <v>3.2706102464421107E-2</v>
       </c>
       <c r="DI6" t="s">
-        <v>181</v>
+        <v>204</v>
       </c>
       <c r="DJ6">
         <v>0.89087499999999997</v>
@@ -3667,7 +3680,7 @@
         <v>3.2473073903518959E-2</v>
       </c>
       <c r="EB6" t="s">
-        <v>181</v>
+        <v>204</v>
       </c>
       <c r="EC6">
         <v>0.89087499999999997</v>
@@ -3717,10 +3730,10 @@
     </row>
     <row r="7" spans="1:147" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>178</v>
+        <v>170</v>
       </c>
       <c r="B7" t="s">
-        <v>182</v>
+        <v>173</v>
       </c>
       <c r="C7">
         <v>8.7750000000000004</v>
@@ -3741,10 +3754,10 @@
         <v>149</v>
       </c>
       <c r="I7" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="J7" t="s">
-        <v>183</v>
+        <v>174</v>
       </c>
       <c r="K7" t="s">
         <v>149</v>
@@ -3759,7 +3772,7 @@
         <v>149</v>
       </c>
       <c r="O7" t="s">
-        <v>184</v>
+        <v>175</v>
       </c>
       <c r="P7" t="s">
         <v>149</v>
@@ -3855,7 +3868,7 @@
         <v>8.2371763027551059E-2</v>
       </c>
       <c r="AU7">
-        <v>8.0796027239735807E-2</v>
+        <v>8.4142779504455034E-2</v>
       </c>
       <c r="AV7" t="s">
         <v>149</v>
@@ -3903,7 +3916,7 @@
         <v>9.9292320125346972E-2</v>
       </c>
       <c r="BK7" t="s">
-        <v>169</v>
+        <v>196</v>
       </c>
       <c r="BL7">
         <v>0.91225000000000001</v>
@@ -3948,7 +3961,7 @@
         <v>9.9292320125346972E-2</v>
       </c>
       <c r="BZ7" t="s">
-        <v>169</v>
+        <v>196</v>
       </c>
       <c r="CA7">
         <v>0.92644318780291768</v>
@@ -4053,7 +4066,7 @@
         <v>6.992047400278309E-2</v>
       </c>
       <c r="DI7" t="s">
-        <v>181</v>
+        <v>204</v>
       </c>
       <c r="DJ7">
         <v>0.86837500000000001</v>
@@ -4110,7 +4123,7 @@
         <v>6.9685495410532525E-2</v>
       </c>
       <c r="EB7" t="s">
-        <v>181</v>
+        <v>204</v>
       </c>
       <c r="EC7">
         <v>0.86837500000000001</v>
@@ -4160,10 +4173,10 @@
     </row>
     <row r="8" spans="1:147" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>182</v>
+        <v>173</v>
       </c>
       <c r="B8" t="s">
-        <v>185</v>
+        <v>176</v>
       </c>
       <c r="C8">
         <v>10.275</v>
@@ -4187,7 +4200,7 @@
         <v>150</v>
       </c>
       <c r="J8" t="s">
-        <v>186</v>
+        <v>177</v>
       </c>
       <c r="K8" t="s">
         <v>149</v>
@@ -4202,7 +4215,7 @@
         <v>149</v>
       </c>
       <c r="O8" t="s">
-        <v>187</v>
+        <v>178</v>
       </c>
       <c r="P8" t="s">
         <v>149</v>
@@ -4298,10 +4311,10 @@
         <v>0.12476333234780576</v>
       </c>
       <c r="AU8">
-        <v>0.14369650497165254</v>
+        <v>0.14704325723637179</v>
       </c>
       <c r="AV8" t="s">
-        <v>188</v>
+        <v>179</v>
       </c>
       <c r="AW8">
         <v>0.89174999999999993</v>
@@ -4346,7 +4359,7 @@
         <v>0.1621927978572637</v>
       </c>
       <c r="BK8" t="s">
-        <v>169</v>
+        <v>196</v>
       </c>
       <c r="BL8">
         <v>0.89174999999999993</v>
@@ -4391,7 +4404,7 @@
         <v>0.1621927978572637</v>
       </c>
       <c r="BZ8" t="s">
-        <v>169</v>
+        <v>196</v>
       </c>
       <c r="CA8">
         <v>0.89926958306060345</v>
@@ -4496,7 +4509,7 @@
         <v>0.13287145957449412</v>
       </c>
       <c r="DI8" t="s">
-        <v>198</v>
+        <v>205</v>
       </c>
       <c r="DJ8">
         <v>0.84587499999999993</v>
@@ -4553,7 +4566,7 @@
         <v>0.13255569980673132</v>
       </c>
       <c r="EB8" t="s">
-        <v>198</v>
+        <v>205</v>
       </c>
       <c r="EC8">
         <v>0.84587499999999993</v>
@@ -4603,10 +4616,10 @@
     </row>
     <row r="9" spans="1:147" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>185</v>
+        <v>176</v>
       </c>
       <c r="B9" t="s">
-        <v>189</v>
+        <v>180</v>
       </c>
       <c r="C9">
         <v>11.775</v>
@@ -4645,7 +4658,7 @@
         <v>149</v>
       </c>
       <c r="O9" t="s">
-        <v>190</v>
+        <v>181</v>
       </c>
       <c r="P9" t="s">
         <v>149</v>
@@ -4741,10 +4754,10 @@
         <v>0.16576607722289835</v>
       </c>
       <c r="AU9">
-        <v>0.20471277263679655</v>
+        <v>0.2080595249015158</v>
       </c>
       <c r="AV9" t="s">
-        <v>191</v>
+        <v>182</v>
       </c>
       <c r="AW9">
         <v>0.84674999999999989</v>
@@ -4789,7 +4802,7 @@
         <v>0.22320906552240771</v>
       </c>
       <c r="BK9" t="s">
-        <v>169</v>
+        <v>196</v>
       </c>
       <c r="BL9">
         <v>0.84674999999999989</v>
@@ -4834,7 +4847,7 @@
         <v>0.22320906552240771</v>
       </c>
       <c r="BZ9" t="s">
-        <v>169</v>
+        <v>196</v>
       </c>
       <c r="CA9">
         <v>0.86277342574087035</v>
@@ -4939,7 +4952,7 @@
         <v>0.19429252871199848</v>
       </c>
       <c r="DI9" t="s">
-        <v>198</v>
+        <v>205</v>
       </c>
       <c r="DJ9">
         <v>0.82337499999999997</v>
@@ -4996,7 +5009,7 @@
         <v>0.13782576161403962</v>
       </c>
       <c r="EB9" t="s">
-        <v>198</v>
+        <v>205</v>
       </c>
       <c r="EC9">
         <v>0.82337499999999997</v>
@@ -5046,10 +5059,10 @@
     </row>
     <row r="10" spans="1:147" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>189</v>
+        <v>180</v>
       </c>
       <c r="B10" t="s">
-        <v>192</v>
+        <v>183</v>
       </c>
       <c r="C10">
         <v>13.275</v>
@@ -5073,7 +5086,7 @@
         <v>150</v>
       </c>
       <c r="J10" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="K10" t="s">
         <v>149</v>
@@ -5088,7 +5101,7 @@
         <v>149</v>
       </c>
       <c r="O10" t="s">
-        <v>193</v>
+        <v>184</v>
       </c>
       <c r="P10" t="s">
         <v>149</v>
@@ -5184,10 +5197,10 @@
         <v>0.20542471790128181</v>
       </c>
       <c r="AU10">
-        <v>0.26390602081287823</v>
+        <v>0.26725277307759748</v>
       </c>
       <c r="AV10" t="s">
-        <v>194</v>
+        <v>185</v>
       </c>
       <c r="AW10">
         <v>0.80174999999999996</v>
@@ -5232,7 +5245,7 @@
         <v>0.28240231369848939</v>
       </c>
       <c r="BK10" t="s">
-        <v>169</v>
+        <v>196</v>
       </c>
       <c r="BL10">
         <v>0.80174999999999996</v>
@@ -5277,7 +5290,7 @@
         <v>0.28240231369848939</v>
       </c>
       <c r="BZ10" t="s">
-        <v>169</v>
+        <v>196</v>
       </c>
       <c r="CA10">
         <v>0.81793229677798485</v>
@@ -5382,7 +5395,7 @@
         <v>0.2543361373704861</v>
       </c>
       <c r="DI10" t="s">
-        <v>198</v>
+        <v>205</v>
       </c>
       <c r="DJ10">
         <v>0.800875</v>
@@ -5439,7 +5452,7 @@
         <v>0.13782576161403962</v>
       </c>
       <c r="EB10" t="s">
-        <v>198</v>
+        <v>205</v>
       </c>
       <c r="EC10">
         <v>0.800875</v>
@@ -5489,10 +5502,10 @@
     </row>
     <row r="11" spans="1:147" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>192</v>
+        <v>183</v>
       </c>
       <c r="B11" t="s">
-        <v>195</v>
+        <v>186</v>
       </c>
       <c r="C11">
         <v>14.775</v>
@@ -5513,7 +5526,7 @@
         <v>149</v>
       </c>
       <c r="I11" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="J11" t="s">
         <v>151</v>
@@ -5531,7 +5544,7 @@
         <v>149</v>
       </c>
       <c r="O11" t="s">
-        <v>196</v>
+        <v>187</v>
       </c>
       <c r="P11" t="s">
         <v>149</v>
@@ -5627,10 +5640,10 @@
         <v>0.24862955474715293</v>
       </c>
       <c r="AU11">
-        <v>0.32798174121311996</v>
+        <v>0.33132849347783921</v>
       </c>
       <c r="AV11" t="s">
-        <v>197</v>
+        <v>188</v>
       </c>
       <c r="AW11">
         <v>0.75675000000000003</v>
@@ -5675,7 +5688,7 @@
         <v>0.34647803409873112</v>
       </c>
       <c r="BK11" t="s">
-        <v>169</v>
+        <v>196</v>
       </c>
       <c r="BL11">
         <v>0.75675000000000003</v>
@@ -5720,7 +5733,7 @@
         <v>0.34647803409873112</v>
       </c>
       <c r="BZ11" t="s">
-        <v>169</v>
+        <v>196</v>
       </c>
       <c r="CA11">
         <v>0.76831019922745336</v>
@@ -5825,7 +5838,7 @@
         <v>0.31951297522423061</v>
       </c>
       <c r="DI11" t="s">
-        <v>198</v>
+        <v>205</v>
       </c>
       <c r="DJ11">
         <v>0.77837500000000004</v>
@@ -5882,7 +5895,7 @@
         <v>0.20300259946778412</v>
       </c>
       <c r="EB11" t="s">
-        <v>198</v>
+        <v>205</v>
       </c>
       <c r="EC11">
         <v>0.77837500000000004</v>
@@ -5932,10 +5945,10 @@
     </row>
     <row r="12" spans="1:147" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>195</v>
+        <v>186</v>
       </c>
       <c r="B12" t="s">
-        <v>199</v>
+        <v>189</v>
       </c>
       <c r="C12">
         <v>16.274999999999999</v>
@@ -5956,10 +5969,10 @@
         <v>149</v>
       </c>
       <c r="I12" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="J12" t="s">
-        <v>200</v>
+        <v>190</v>
       </c>
       <c r="K12" t="s">
         <v>149</v>
@@ -5974,7 +5987,7 @@
         <v>149</v>
       </c>
       <c r="O12" t="s">
-        <v>201</v>
+        <v>191</v>
       </c>
       <c r="P12" t="s">
         <v>149</v>
@@ -6001,7 +6014,7 @@
         <v>149</v>
       </c>
       <c r="X12" t="s">
-        <v>202</v>
+        <v>192</v>
       </c>
       <c r="Y12" t="s">
         <v>149</v>
@@ -6070,7 +6083,7 @@
         <v>0.24862955474715293</v>
       </c>
       <c r="AU12">
-        <v>0.32798174121311996</v>
+        <v>0.33132849347783921</v>
       </c>
       <c r="AV12" t="s">
         <v>149</v>
@@ -6268,7 +6281,7 @@
         <v>0.31951297522423061</v>
       </c>
       <c r="DI12" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
       <c r="DJ12" t="s">
         <v>149</v>
@@ -6325,7 +6338,7 @@
         <v>0.20300259946778412</v>
       </c>
       <c r="EB12" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
       <c r="EC12" t="s">
         <v>149</v>
@@ -6375,10 +6388,10 @@
     </row>
     <row r="13" spans="1:147" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>199</v>
+        <v>189</v>
       </c>
       <c r="B13" t="s">
-        <v>203</v>
+        <v>193</v>
       </c>
       <c r="C13">
         <v>17.774999999999999</v>
@@ -6399,10 +6412,10 @@
         <v>149</v>
       </c>
       <c r="I13" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="J13" t="s">
-        <v>200</v>
+        <v>190</v>
       </c>
       <c r="K13" t="s">
         <v>149</v>
@@ -6417,7 +6430,7 @@
         <v>149</v>
       </c>
       <c r="O13" t="s">
-        <v>204</v>
+        <v>194</v>
       </c>
       <c r="P13" t="s">
         <v>149</v>
@@ -6444,7 +6457,7 @@
         <v>149</v>
       </c>
       <c r="X13" t="s">
-        <v>180</v>
+        <v>172</v>
       </c>
       <c r="Y13" t="s">
         <v>149</v>
@@ -6513,7 +6526,7 @@
         <v>0.24862955474715293</v>
       </c>
       <c r="AU13">
-        <v>0.32798174121311996</v>
+        <v>0.33132849347783921</v>
       </c>
       <c r="AV13" t="s">
         <v>149</v>
@@ -6711,7 +6724,7 @@
         <v>0.31951297522423061</v>
       </c>
       <c r="DI13" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
       <c r="DJ13" t="s">
         <v>149</v>
@@ -6768,7 +6781,7 @@
         <v>0.20300259946778412</v>
       </c>
       <c r="EB13" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
       <c r="EC13" t="s">
         <v>149</v>
@@ -6818,10 +6831,10 @@
     </row>
     <row r="14" spans="1:147" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>203</v>
+        <v>193</v>
       </c>
       <c r="B14" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C14">
         <v>19.262499999999999</v>
@@ -6842,10 +6855,10 @@
         <v>149</v>
       </c>
       <c r="I14" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="J14" t="s">
-        <v>186</v>
+        <v>177</v>
       </c>
       <c r="K14" t="s">
         <v>149</v>
@@ -6860,7 +6873,7 @@
         <v>149</v>
       </c>
       <c r="O14" t="s">
-        <v>205</v>
+        <v>195</v>
       </c>
       <c r="P14" t="s">
         <v>149</v>
@@ -6887,7 +6900,7 @@
         <v>149</v>
       </c>
       <c r="X14" t="s">
-        <v>184</v>
+        <v>175</v>
       </c>
       <c r="Y14" t="s">
         <v>149</v>
@@ -6956,7 +6969,7 @@
         <v>0.24862955474715293</v>
       </c>
       <c r="AU14">
-        <v>0.32798174121311996</v>
+        <v>0.33132849347783921</v>
       </c>
       <c r="AV14" t="s">
         <v>149</v>
@@ -7154,7 +7167,7 @@
         <v>0.31951297522423061</v>
       </c>
       <c r="DI14" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
       <c r="DJ14" t="s">
         <v>149</v>
@@ -7211,7 +7224,7 @@
         <v>0.20300259946778412</v>
       </c>
       <c r="EB14" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
       <c r="EC14" t="s">
         <v>149</v>
@@ -7270,7 +7283,7 @@
   <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
@@ -7280,7 +7293,8 @@
     <col min="4" max="4" width="14" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="16.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="8.88671875" style="1"/>
+    <col min="8" max="8" width="9.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.3">
@@ -7376,7 +7390,7 @@
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <f>mat!AP4</f>
-        <v>10</v>
+        <v>1.447489501698765</v>
       </c>
       <c r="B4" s="1">
         <f>mat!BE4</f>
@@ -7406,7 +7420,7 @@
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <f>mat!AP5</f>
-        <v>10</v>
+        <v>1.4570710427751399</v>
       </c>
       <c r="B5" s="1">
         <f>mat!BE5</f>
@@ -7711,12 +7725,456 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70FB19C2-6DC8-4DF4-BE04-94333A556EA5}">
+  <dimension ref="A1:G15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I14" sqref="I14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="12.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="15.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="16.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="8.88671875" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="str">
+        <f>mat!AS1</f>
+        <v>sptSeed-PL</v>
+      </c>
+      <c r="B1" s="3" t="str">
+        <f>mat!BH1</f>
+        <v>sptHBF2012-PL</v>
+      </c>
+      <c r="C1" s="3" t="str">
+        <f>mat!BW1</f>
+        <v>sptHBF2017-PL</v>
+      </c>
+      <c r="D1" s="3" t="str">
+        <f>mat!CM1</f>
+        <v>sptNCEER-PL</v>
+      </c>
+      <c r="E1" s="3" t="str">
+        <f>mat!DF1</f>
+        <v>sptNJRA1996-PL</v>
+      </c>
+      <c r="F1" s="3" t="str">
+        <f>mat!DY1</f>
+        <v>sptNJRA2017-PL</v>
+      </c>
+      <c r="G1" s="3" t="str">
+        <f>mat!EN1</f>
+        <v>sptTY-PL</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" s="5">
+        <f>mat!AS2</f>
+        <v>1.3177443014899113</v>
+      </c>
+      <c r="B2" s="5">
+        <f>mat!BH2</f>
+        <v>2.7102559354828508</v>
+      </c>
+      <c r="C2" s="5">
+        <f>mat!BW2</f>
+        <v>2.7102559354828508</v>
+      </c>
+      <c r="D2" s="5">
+        <f>mat!CM2</f>
+        <v>6.3555296672182804</v>
+      </c>
+      <c r="E2" s="5">
+        <f>mat!DF2</f>
+        <v>0</v>
+      </c>
+      <c r="F2" s="5">
+        <f>mat!DY2</f>
+        <v>0</v>
+      </c>
+      <c r="G2" s="5">
+        <f>mat!EN2</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" s="5">
+        <f>mat!AS3</f>
+        <v>1.3177443014899113</v>
+      </c>
+      <c r="B3" s="5">
+        <f>mat!BH3</f>
+        <v>2.7102559354828508</v>
+      </c>
+      <c r="C3" s="5">
+        <f>mat!BW3</f>
+        <v>2.7102559354828508</v>
+      </c>
+      <c r="D3" s="5">
+        <f>mat!CM3</f>
+        <v>6.3555296672182804</v>
+      </c>
+      <c r="E3" s="5">
+        <f>mat!DF3</f>
+        <v>0</v>
+      </c>
+      <c r="F3" s="5">
+        <f>mat!DY3</f>
+        <v>0</v>
+      </c>
+      <c r="G3" s="5">
+        <f>mat!EN3</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" s="5">
+        <f>mat!AS4</f>
+        <v>1.3177443014899113</v>
+      </c>
+      <c r="B4" s="5">
+        <f>mat!BH4</f>
+        <v>2.7102559354828508</v>
+      </c>
+      <c r="C4" s="5">
+        <f>mat!BW4</f>
+        <v>2.7102559354828508</v>
+      </c>
+      <c r="D4" s="5">
+        <f>mat!CM4</f>
+        <v>6.3555296672182804</v>
+      </c>
+      <c r="E4" s="5">
+        <f>mat!DF4</f>
+        <v>0</v>
+      </c>
+      <c r="F4" s="5">
+        <f>mat!DY4</f>
+        <v>0</v>
+      </c>
+      <c r="G4" s="5">
+        <f>mat!EN4</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" s="5">
+        <f>mat!AS5</f>
+        <v>1.3177443014899113</v>
+      </c>
+      <c r="B5" s="5">
+        <f>mat!BH5</f>
+        <v>2.7102559354828508</v>
+      </c>
+      <c r="C5" s="5">
+        <f>mat!BW5</f>
+        <v>2.7102559354828508</v>
+      </c>
+      <c r="D5" s="5">
+        <f>mat!CM5</f>
+        <v>6.3555296672182804</v>
+      </c>
+      <c r="E5" s="5">
+        <f>mat!DF5</f>
+        <v>0</v>
+      </c>
+      <c r="F5" s="5">
+        <f>mat!DY5</f>
+        <v>0</v>
+      </c>
+      <c r="G5" s="5">
+        <f>mat!EN5</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" s="5">
+        <f>mat!AS6</f>
+        <v>1.3177443014899113</v>
+      </c>
+      <c r="B6" s="5">
+        <f>mat!BH6</f>
+        <v>2.7102559354828508</v>
+      </c>
+      <c r="C6" s="5">
+        <f>mat!BW6</f>
+        <v>2.7102559354828508</v>
+      </c>
+      <c r="D6" s="5">
+        <f>mat!CM6</f>
+        <v>8.1659105649176862</v>
+      </c>
+      <c r="E6" s="5">
+        <f>mat!DF6</f>
+        <v>4.0652182879099241</v>
+      </c>
+      <c r="F6" s="5">
+        <f>mat!DY6</f>
+        <v>3.5412755035767671</v>
+      </c>
+      <c r="G6" s="5">
+        <f>mat!EN6</f>
+        <v>1.359274389521586</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" s="5">
+        <f>mat!AS7</f>
+        <v>3.7886225893923928</v>
+      </c>
+      <c r="B7" s="5">
+        <f>mat!BH7</f>
+        <v>5.3627276362466603</v>
+      </c>
+      <c r="C7" s="5">
+        <f>mat!BW7</f>
+        <v>5.3627276362466603</v>
+      </c>
+      <c r="D7" s="5">
+        <f>mat!CM7</f>
+        <v>11.249443972923423</v>
+      </c>
+      <c r="E7" s="5">
+        <f>mat!DF7</f>
+        <v>8.2517440041643404</v>
+      </c>
+      <c r="F7" s="5">
+        <f>mat!DY7</f>
+        <v>7.6250376867402707</v>
+      </c>
+      <c r="G7" s="5">
+        <f>mat!EN7</f>
+        <v>4.3293539421777467</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8" s="5">
+        <f>mat!AS8</f>
+        <v>7.4075091884809225</v>
+      </c>
+      <c r="B8" s="5">
+        <f>mat!BH8</f>
+        <v>9.8910545574253437</v>
+      </c>
+      <c r="C8" s="5">
+        <f>mat!BW8</f>
+        <v>9.8910545574253437</v>
+      </c>
+      <c r="D8" s="5">
+        <f>mat!CM8</f>
+        <v>15.374734232213081</v>
+      </c>
+      <c r="E8" s="5">
+        <f>mat!DF8</f>
+        <v>12.063088557916332</v>
+      </c>
+      <c r="F8" s="5">
+        <f>mat!DY8</f>
+        <v>8.4297866578328584</v>
+      </c>
+      <c r="G8" s="5">
+        <f>mat!EN8</f>
+        <v>8.1767583096783891</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9" s="5">
+        <f>mat!AS9</f>
+        <v>10.179207762418445</v>
+      </c>
+      <c r="B9" s="5">
+        <f>mat!BH9</f>
+        <v>13.468193083105273</v>
+      </c>
+      <c r="C9" s="5">
+        <f>mat!BW9</f>
+        <v>13.468193083105273</v>
+      </c>
+      <c r="D9" s="5">
+        <f>mat!CM9</f>
+        <v>18.626096230705784</v>
+      </c>
+      <c r="E9" s="5">
+        <f>mat!DF9</f>
+        <v>15.096813006406498</v>
+      </c>
+      <c r="F9" s="5">
+        <f>mat!DY9</f>
+        <v>8.4297866578328584</v>
+      </c>
+      <c r="G9" s="5">
+        <f>mat!EN9</f>
+        <v>11.271584901406168</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10" s="5">
+        <f>mat!AS10</f>
+        <v>12.143573441023193</v>
+      </c>
+      <c r="B10" s="5">
+        <f>mat!BH10</f>
+        <v>16.153796664402108</v>
+      </c>
+      <c r="C10" s="5">
+        <f>mat!BW10</f>
+        <v>16.153796664402108</v>
+      </c>
+      <c r="D10" s="5">
+        <f>mat!CM10</f>
+        <v>21.054289299192828</v>
+      </c>
+      <c r="E10" s="5">
+        <f>mat!DF10</f>
+        <v>17.401767146748327</v>
+      </c>
+      <c r="F10" s="5">
+        <f>mat!DY10</f>
+        <v>8.4297866578328584</v>
+      </c>
+      <c r="G10" s="5">
+        <f>mat!EN10</f>
+        <v>13.656161208355044</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11" s="5">
+        <f>mat!AS11</f>
+        <v>13.94428675809394</v>
+      </c>
+      <c r="B11" s="5">
+        <f>mat!BH11</f>
+        <v>18.407363763128849</v>
+      </c>
+      <c r="C11" s="5">
+        <f>mat!BW11</f>
+        <v>18.407363763128849</v>
+      </c>
+      <c r="D11" s="5">
+        <f>mat!CM11</f>
+        <v>23.045949315149091</v>
+      </c>
+      <c r="E11" s="5">
+        <f>mat!DF11</f>
+        <v>19.458298774392677</v>
+      </c>
+      <c r="F11" s="5">
+        <f>mat!DY11</f>
+        <v>10.056687713200068</v>
+      </c>
+      <c r="G11" s="5">
+        <f>mat!EN11</f>
+        <v>15.678989260651788</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A12" s="5">
+        <f>mat!AS12</f>
+        <v>13.94428675809394</v>
+      </c>
+      <c r="B12" s="5">
+        <f>mat!BH12</f>
+        <v>18.407363763128849</v>
+      </c>
+      <c r="C12" s="5">
+        <f>mat!BW12</f>
+        <v>18.407363763128849</v>
+      </c>
+      <c r="D12" s="5">
+        <f>mat!CM12</f>
+        <v>23.045949315149091</v>
+      </c>
+      <c r="E12" s="5">
+        <f>mat!DF12</f>
+        <v>19.458298774392677</v>
+      </c>
+      <c r="F12" s="5">
+        <f>mat!DY12</f>
+        <v>10.056687713200068</v>
+      </c>
+      <c r="G12" s="5">
+        <f>mat!EN12</f>
+        <v>15.678989260651788</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A13" s="5">
+        <f>mat!AS13</f>
+        <v>13.94428675809394</v>
+      </c>
+      <c r="B13" s="5">
+        <f>mat!BH13</f>
+        <v>18.407363763128849</v>
+      </c>
+      <c r="C13" s="5">
+        <f>mat!BW13</f>
+        <v>18.407363763128849</v>
+      </c>
+      <c r="D13" s="5">
+        <f>mat!CM13</f>
+        <v>23.045949315149091</v>
+      </c>
+      <c r="E13" s="5">
+        <f>mat!DF13</f>
+        <v>19.458298774392677</v>
+      </c>
+      <c r="F13" s="5">
+        <f>mat!DY13</f>
+        <v>10.056687713200068</v>
+      </c>
+      <c r="G13" s="5">
+        <f>mat!EN13</f>
+        <v>15.678989260651788</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A14" s="4">
+        <f>mat!AS14</f>
+        <v>13.94428675809394</v>
+      </c>
+      <c r="B14" s="4">
+        <f>mat!BH14</f>
+        <v>18.407363763128849</v>
+      </c>
+      <c r="C14" s="4">
+        <f>mat!BW14</f>
+        <v>18.407363763128849</v>
+      </c>
+      <c r="D14" s="4">
+        <f>mat!CM14</f>
+        <v>23.045949315149091</v>
+      </c>
+      <c r="E14" s="4">
+        <f>mat!DF14</f>
+        <v>19.458298774392677</v>
+      </c>
+      <c r="F14" s="4">
+        <f>mat!DY14</f>
+        <v>10.056687713200068</v>
+      </c>
+      <c r="G14" s="4">
+        <f>mat!EN14</f>
+        <v>15.678989260651788</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3"/>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01A24ED4-848D-44FB-9EE4-1892B20FDD58}">
   <dimension ref="A1:I104"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C66" sqref="C66"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
   <cols>
@@ -7853,11 +8311,11 @@
       </c>
       <c r="B4" s="1">
         <f>mat!AO4</f>
-        <v>18.765665696998305</v>
+        <v>0.6</v>
       </c>
       <c r="C4" s="1">
         <f>mat!AP4</f>
-        <v>10</v>
+        <v>1.447489501698765</v>
       </c>
       <c r="D4" s="1">
         <f>mat!AQ4</f>
@@ -7865,7 +8323,7 @@
       </c>
       <c r="E4" s="1">
         <f>mat!AR4</f>
-        <v>0</v>
+        <v>0.11307814700732616</v>
       </c>
       <c r="F4" s="1">
         <f>mat!AS4</f>
@@ -7877,11 +8335,11 @@
       </c>
       <c r="H4" s="1">
         <f>mat!AU4</f>
-        <v>3.4896234280900613E-2</v>
+        <v>3.6592406486010504E-2</v>
       </c>
       <c r="I4" s="1" t="str">
         <f>mat!AV4</f>
-        <v>Volumetric Strain(Tokimatsu And Seed): 出現外插情形 N160=38.29626079871692 &gt; N160Max=33.845439845659584，依照CSR=0.4145107783481977並給予最小體積應變vstr=0.1%, Volumetric Strain(Ishihara And Yoshimine): 出現外插情形 N172=31.913550665597437 &gt; N172Max=30，依照FS=2並給予最小體積應變vstr=0%</v>
+        <v>CRR75[18.765665696998305]大於0.6超過原研究範疇，強制改為0.6; Volumetric Strain(Tokimatsu And Seed): 出現外插情形 N160=38.29626079871692 &gt; N160Max=33.845439845659584，依照CSR=0.4145107783481977並給予最小體積應變vstr=0.1%; Volumetric Strain(Ishihara And Yoshimine): 出現外插情形 N172=31.913550665597437 &gt; N172Max=30，依照FS=1.447489501698765並給予最小體積應變vstr=0.11307814700732616%</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
@@ -7891,11 +8349,11 @@
       </c>
       <c r="B5" s="1">
         <f>mat!AO5</f>
-        <v>17.238576542916931</v>
+        <v>0.6</v>
       </c>
       <c r="C5" s="1">
         <f>mat!AP5</f>
-        <v>10</v>
+        <v>1.4570710427751399</v>
       </c>
       <c r="D5" s="1">
         <f>mat!AQ5</f>
@@ -7903,7 +8361,7 @@
       </c>
       <c r="E5" s="1">
         <f>mat!AR5</f>
-        <v>0</v>
+        <v>0.11003867064062244</v>
       </c>
       <c r="F5" s="1">
         <f>mat!AS5</f>
@@ -7915,11 +8373,11 @@
       </c>
       <c r="H5" s="1">
         <f>mat!AU5</f>
-        <v>3.4896234280900613E-2</v>
+        <v>3.8242986545619841E-2</v>
       </c>
       <c r="I5" s="1" t="str">
         <f>mat!AV5</f>
-        <v>Volumetric Strain(Tokimatsu And Seed): 出現外插情形 N160=38.07293279469695 &gt; N160Max=33.752136934605055，依照CSR=0.4117850004466762並給予最小體積應變vstr=0.1%, Volumetric Strain(Ishihara And Yoshimine): 出現外插情形 N172=31.727443995580796 &gt; N172Max=30，依照FS=2並給予最小體積應變vstr=0%</v>
+        <v>CRR75[17.23857654291693]大於0.6超過原研究範疇，強制改為0.6; Volumetric Strain(Tokimatsu And Seed): 出現外插情形 N160=38.07293279469695 &gt; N160Max=33.752136934605055，依照CSR=0.4117850004466762並給予最小體積應變vstr=0.1%; Volumetric Strain(Ishihara And Yoshimine): 出現外插情形 N172=31.727443995580796 &gt; N172Max=30，依照FS=1.4570710427751399並給予最小體積應變vstr=0.11003867064062244%</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
@@ -7953,7 +8411,7 @@
       </c>
       <c r="H6" s="1">
         <f>mat!AU6</f>
-        <v>4.4079123330625233E-2</v>
+        <v>4.7425875595344461E-2</v>
       </c>
       <c r="I6" s="1" t="str">
         <f>mat!AV6</f>
@@ -7991,7 +8449,7 @@
       </c>
       <c r="H7" s="1">
         <f>mat!AU7</f>
-        <v>8.0796027239735807E-2</v>
+        <v>8.4142779504455034E-2</v>
       </c>
       <c r="I7" s="1" t="str">
         <f>mat!AV7</f>
@@ -8029,7 +8487,7 @@
       </c>
       <c r="H8" s="1">
         <f>mat!AU8</f>
-        <v>0.14369650497165254</v>
+        <v>0.14704325723637179</v>
       </c>
       <c r="I8" s="1" t="str">
         <f>mat!AV8</f>
@@ -8067,7 +8525,7 @@
       </c>
       <c r="H9" s="1">
         <f>mat!AU9</f>
-        <v>0.20471277263679655</v>
+        <v>0.2080595249015158</v>
       </c>
       <c r="I9" s="1" t="str">
         <f>mat!AV9</f>
@@ -8105,7 +8563,7 @@
       </c>
       <c r="H10" s="1">
         <f>mat!AU10</f>
-        <v>0.26390602081287823</v>
+        <v>0.26725277307759748</v>
       </c>
       <c r="I10" s="1" t="str">
         <f>mat!AV10</f>
@@ -8143,7 +8601,7 @@
       </c>
       <c r="H11" s="1">
         <f>mat!AU11</f>
-        <v>0.32798174121311996</v>
+        <v>0.33132849347783921</v>
       </c>
       <c r="I11" s="1" t="str">
         <f>mat!AV11</f>
@@ -8181,7 +8639,7 @@
       </c>
       <c r="H12" s="1">
         <f>mat!AU12</f>
-        <v>0.32798174121311996</v>
+        <v>0.33132849347783921</v>
       </c>
       <c r="I12" s="1" t="str">
         <f>mat!AV12</f>
@@ -8219,7 +8677,7 @@
       </c>
       <c r="H13" s="1">
         <f>mat!AU13</f>
-        <v>0.32798174121311996</v>
+        <v>0.33132849347783921</v>
       </c>
       <c r="I13" s="1" t="str">
         <f>mat!AV13</f>
@@ -8257,7 +8715,7 @@
       </c>
       <c r="H14" s="1">
         <f>mat!AU14</f>
-        <v>0.32798174121311996</v>
+        <v>0.33132849347783921</v>
       </c>
       <c r="I14" s="1" t="str">
         <f>mat!AV14</f>
@@ -8413,7 +8871,7 @@
       </c>
       <c r="I19" s="1" t="str">
         <f>mat!BK4</f>
-        <v>PI 非數字與非NP，略過部份非液化條件檢核</v>
+        <v/>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.3">
@@ -8451,7 +8909,7 @@
       </c>
       <c r="I20" s="1" t="str">
         <f>mat!BK5</f>
-        <v>PI 非數字與非NP，略過部份非液化條件檢核</v>
+        <v/>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.3">
@@ -8489,7 +8947,7 @@
       </c>
       <c r="I21" s="1" t="str">
         <f>mat!BK6</f>
-        <v>PI 非數字與非NP，略過部份非液化條件檢核</v>
+        <v>PI非數字與非NP，強制略過部份非液化條件檢核</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.3">
@@ -8527,7 +8985,7 @@
       </c>
       <c r="I22" s="1" t="str">
         <f>mat!BK7</f>
-        <v>PI 非數字與非NP，略過部份非液化條件檢核</v>
+        <v>PI非數字與非NP，強制略過部份非液化條件檢核</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.3">
@@ -8565,7 +9023,7 @@
       </c>
       <c r="I23" s="1" t="str">
         <f>mat!BK8</f>
-        <v>PI 非數字與非NP，略過部份非液化條件檢核</v>
+        <v>PI非數字與非NP，強制略過部份非液化條件檢核</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.3">
@@ -8603,7 +9061,7 @@
       </c>
       <c r="I24" s="1" t="str">
         <f>mat!BK9</f>
-        <v>PI 非數字與非NP，略過部份非液化條件檢核</v>
+        <v>PI非數字與非NP，強制略過部份非液化條件檢核</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.3">
@@ -8641,7 +9099,7 @@
       </c>
       <c r="I25" s="1" t="str">
         <f>mat!BK10</f>
-        <v>PI 非數字與非NP，略過部份非液化條件檢核</v>
+        <v>PI非數字與非NP，強制略過部份非液化條件檢核</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.3">
@@ -8679,7 +9137,7 @@
       </c>
       <c r="I26" s="1" t="str">
         <f>mat!BK11</f>
-        <v>PI 非數字與非NP，略過部份非液化條件檢核</v>
+        <v>PI非數字與非NP，強制略過部份非液化條件檢核</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.3">
@@ -8945,7 +9403,7 @@
       </c>
       <c r="I34" s="1" t="str">
         <f>mat!BZ4</f>
-        <v>PI 非數字與非NP，略過部份非液化條件檢核</v>
+        <v/>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.3">
@@ -8983,7 +9441,7 @@
       </c>
       <c r="I35" s="1" t="str">
         <f>mat!BZ5</f>
-        <v>PI 非數字與非NP，略過部份非液化條件檢核</v>
+        <v/>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.3">
@@ -9021,7 +9479,7 @@
       </c>
       <c r="I36" s="1" t="str">
         <f>mat!BZ6</f>
-        <v>PI 非數字與非NP，略過部份非液化條件檢核</v>
+        <v>PI非數字與非NP，強制略過部份非液化條件檢核</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.3">
@@ -9059,7 +9517,7 @@
       </c>
       <c r="I37" s="1" t="str">
         <f>mat!BZ7</f>
-        <v>PI 非數字與非NP，略過部份非液化條件檢核</v>
+        <v>PI非數字與非NP，強制略過部份非液化條件檢核</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.3">
@@ -9097,7 +9555,7 @@
       </c>
       <c r="I38" s="1" t="str">
         <f>mat!BZ8</f>
-        <v>PI 非數字與非NP，略過部份非液化條件檢核</v>
+        <v>PI非數字與非NP，強制略過部份非液化條件檢核</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.3">
@@ -9135,7 +9593,7 @@
       </c>
       <c r="I39" s="1" t="str">
         <f>mat!BZ9</f>
-        <v>PI 非數字與非NP，略過部份非液化條件檢核</v>
+        <v>PI非數字與非NP，強制略過部份非液化條件檢核</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.3">
@@ -9173,7 +9631,7 @@
       </c>
       <c r="I40" s="1" t="str">
         <f>mat!BZ10</f>
-        <v>PI 非數字與非NP，略過部份非液化條件檢核</v>
+        <v>PI非數字與非NP，強制略過部份非液化條件檢核</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.3">
@@ -9211,7 +9669,7 @@
       </c>
       <c r="I41" s="1" t="str">
         <f>mat!BZ11</f>
-        <v>PI 非數字與非NP，略過部份非液化條件檢核</v>
+        <v>PI非數字與非NP，強制略過部份非液化條件檢核</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.3">
@@ -9933,7 +10391,7 @@
       </c>
       <c r="I62" s="1" t="str">
         <f>mat!DI2</f>
-        <v>D50 非數字，略過部份非液化條件檢核, D10 非數字，略過部份非液化條件檢核, vibrationType 非數字, vibrationType[0] 不等於 1 或 2，更改為預設值1, Volumetric Strain(Tokimatsu And Seed): CSR大於0.6超過原研究範疇，強制改為0.6</v>
+        <v>D50非數字，強制略過部份非液化條件檢核; D10非數字，強制略過部份非液化條件檢核; vibrationType非數字; Volumetric Strain(Tokimatsu And Seed): CSR大於0.6超過原研究範疇，強制改為0.6</v>
       </c>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.3">
@@ -9971,7 +10429,7 @@
       </c>
       <c r="I63" s="1" t="str">
         <f>mat!DI3</f>
-        <v>D50 非數字，略過部份非液化條件檢核, D10 非數字，略過部份非液化條件檢核</v>
+        <v/>
       </c>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.3">
@@ -10009,7 +10467,7 @@
       </c>
       <c r="I64" s="1" t="str">
         <f>mat!DI4</f>
-        <v>D50 非數字，略過部份非液化條件檢核, D10 非數字，略過部份非液化條件檢核, vibrationType 非數字, vibrationType[0] 不等於 1 或 2，更改為預設值1, Volumetric Strain(Tokimatsu And Seed): CSR大於0.6超過原研究範疇，強制改為0.6, Volumetric Strain(Tokimatsu And Seed): 出現外插情形 N160=37.150772494769974 &gt; N160Max=36.7，依照CSR=0.6並給予最小體積應變vstr=0.1%, Volumetric Strain(Ishihara And Yoshimine): 出現外插情形 N172=30.958977078974982 &gt; N172Max=30，依照FS=2並給予最小體積應變vstr=0%</v>
+        <v>D50非數字，強制略過部份非液化條件檢核; D10非數字，強制略過部份非液化條件檢核; vibrationType非數字; Volumetric Strain(Tokimatsu And Seed): CSR大於0.6超過原研究範疇，強制改為0.6; Volumetric Strain(Tokimatsu And Seed): 出現外插情形 N160=37.150772494769974 &gt; N160Max=36.7，依照CSR=0.6並給予最小體積應變vstr=0.1%; Volumetric Strain(Ishihara And Yoshimine): 出現外插情形 N172=30.958977078974982 &gt; N172Max=30，依照FS=2並給予最小體積應變vstr=0%</v>
       </c>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.3">
@@ -10047,7 +10505,7 @@
       </c>
       <c r="I65" s="1" t="str">
         <f>mat!DI5</f>
-        <v>D50 非數字，略過部份非液化條件檢核, D10 非數字，略過部份非液化條件檢核, vibrationType 非數字, vibrationType[0] 不等於 1 或 2，更改為預設值1, Volumetric Strain(Tokimatsu And Seed): CSR大於0.6超過原研究範疇，強制改為0.6, Volumetric Strain(Tokimatsu And Seed): 出現外插情形 N160=38.05808075175254 &gt; N160Max=36.7，依照CSR=0.6並給予最小體積應變vstr=0.1%, Volumetric Strain(Ishihara And Yoshimine): 出現外插情形 N172=31.715067293127117 &gt; N172Max=30，依照FS=2並給予最小體積應變vstr=0%</v>
+        <v>D50非數字，強制略過部份非液化條件檢核; D10非數字，強制略過部份非液化條件檢核; vibrationType非數字; Volumetric Strain(Tokimatsu And Seed): CSR大於0.6超過原研究範疇，強制改為0.6; Volumetric Strain(Tokimatsu And Seed): 出現外插情形 N160=38.05808075175254 &gt; N160Max=36.7，依照CSR=0.6並給予最小體積應變vstr=0.1%; Volumetric Strain(Ishihara And Yoshimine): 出現外插情形 N172=31.715067293127117 &gt; N172Max=30，依照FS=2並給予最小體積應變vstr=0%</v>
       </c>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.3">
@@ -10085,7 +10543,7 @@
       </c>
       <c r="I66" s="1" t="str">
         <f>mat!DI6</f>
-        <v>D50 非數字，略過部份非液化條件檢核, D10 非數字，略過部份非液化條件檢核, vibrationType 非數字, vibrationType[0] 不等於 1 或 2，更改為預設值1</v>
+        <v>D50非數字，強制略過部份非液化條件檢核; D10非數字，強制略過部份非液化條件檢核; vibrationType非數字</v>
       </c>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.3">
@@ -10123,7 +10581,7 @@
       </c>
       <c r="I67" s="1" t="str">
         <f>mat!DI7</f>
-        <v>D50 非數字，略過部份非液化條件檢核, D10 非數字，略過部份非液化條件檢核, vibrationType 非數字, vibrationType[0] 不等於 1 或 2，更改為預設值1</v>
+        <v>D50非數字，強制略過部份非液化條件檢核; D10非數字，強制略過部份非液化條件檢核; vibrationType非數字</v>
       </c>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.3">
@@ -10161,7 +10619,7 @@
       </c>
       <c r="I68" s="1" t="str">
         <f>mat!DI8</f>
-        <v>D50 非數字，略過部份非液化條件檢核, D10 非數字，略過部份非液化條件檢核, PI 非數字與非NP，略過部份非液化條件檢核, vibrationType 非數字, vibrationType[0] 不等於 1 或 2，更改為預設值1</v>
+        <v>PI非數字與非NP，強制略過部份非液化條件檢核; D50非數字，強制略過部份非液化條件檢核; D10非數字，強制略過部份非液化條件檢核; vibrationType非數字</v>
       </c>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.3">
@@ -10199,7 +10657,7 @@
       </c>
       <c r="I69" s="1" t="str">
         <f>mat!DI9</f>
-        <v>D50 非數字，略過部份非液化條件檢核, D10 非數字，略過部份非液化條件檢核, PI 非數字與非NP，略過部份非液化條件檢核, vibrationType 非數字, vibrationType[0] 不等於 1 或 2，更改為預設值1</v>
+        <v>PI非數字與非NP，強制略過部份非液化條件檢核; D50非數字，強制略過部份非液化條件檢核; D10非數字，強制略過部份非液化條件檢核; vibrationType非數字</v>
       </c>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.3">
@@ -10237,7 +10695,7 @@
       </c>
       <c r="I70" s="1" t="str">
         <f>mat!DI10</f>
-        <v>D50 非數字，略過部份非液化條件檢核, D10 非數字，略過部份非液化條件檢核, PI 非數字與非NP，略過部份非液化條件檢核, vibrationType 非數字, vibrationType[0] 不等於 1 或 2，更改為預設值1</v>
+        <v>PI非數字與非NP，強制略過部份非液化條件檢核; D50非數字，強制略過部份非液化條件檢核; D10非數字，強制略過部份非液化條件檢核; vibrationType非數字</v>
       </c>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.3">
@@ -10275,7 +10733,7 @@
       </c>
       <c r="I71" s="1" t="str">
         <f>mat!DI11</f>
-        <v>D50 非數字，略過部份非液化條件檢核, D10 非數字，略過部份非液化條件檢核, PI 非數字與非NP，略過部份非液化條件檢核, vibrationType 非數字, vibrationType[0] 不等於 1 或 2，更改為預設值1</v>
+        <v>PI非數字與非NP，強制略過部份非液化條件檢核; D50非數字，強制略過部份非液化條件檢核; D10非數字，強制略過部份非液化條件檢核; vibrationType非數字</v>
       </c>
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.3">
@@ -10313,7 +10771,7 @@
       </c>
       <c r="I72" s="1" t="str">
         <f>mat!DI12</f>
-        <v>D50 非數字，略過部份非液化條件檢核, D10 非數字，略過部份非液化條件檢核</v>
+        <v/>
       </c>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.3">
@@ -10351,7 +10809,7 @@
       </c>
       <c r="I73" s="1" t="str">
         <f>mat!DI13</f>
-        <v>D50 非數字，略過部份非液化條件檢核, D10 非數字，略過部份非液化條件檢核</v>
+        <v/>
       </c>
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.3">
@@ -10389,7 +10847,7 @@
       </c>
       <c r="I74" s="1" t="str">
         <f>mat!DI14</f>
-        <v>D50 非數字，略過部份非液化條件檢核, D10 非數字，略過部份非液化條件檢核</v>
+        <v/>
       </c>
     </row>
     <row r="76" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
@@ -10465,7 +10923,7 @@
       </c>
       <c r="I77" s="1" t="str">
         <f>mat!EB2</f>
-        <v>D50 非數字，略過部份非液化條件檢核, D10 非數字，略過部份非液化條件檢核, vibrationType 非數字, vibrationType[0] 不等於 1 或 2，更改為預設值1, Volumetric Strain(Tokimatsu And Seed): CSR大於0.6超過原研究範疇，強制改為0.6</v>
+        <v>D50非數字，強制略過部份非液化條件檢核; D10非數字，強制略過部份非液化條件檢核; vibrationType非數字; Volumetric Strain(Tokimatsu And Seed): CSR大於0.6超過原研究範疇，強制改為0.6</v>
       </c>
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.3">
@@ -10503,7 +10961,7 @@
       </c>
       <c r="I78" s="1" t="str">
         <f>mat!EB3</f>
-        <v>D50 非數字，略過部份非液化條件檢核, D10 非數字，略過部份非液化條件檢核</v>
+        <v/>
       </c>
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.3">
@@ -10541,7 +10999,7 @@
       </c>
       <c r="I79" s="1" t="str">
         <f>mat!EB4</f>
-        <v>D50 非數字，略過部份非液化條件檢核, D10 非數字，略過部份非液化條件檢核, vibrationType 非數字, vibrationType[0] 不等於 1 或 2，更改為預設值1, Volumetric Strain(Tokimatsu And Seed): CSR大於0.6超過原研究範疇，強制改為0.6, Volumetric Strain(Tokimatsu And Seed): 出現外插情形 N160=37.150772494769974 &gt; N160Max=36.7，依照CSR=0.6並給予最小體積應變vstr=0.1%, Volumetric Strain(Ishihara And Yoshimine): 出現外插情形 N172=30.958977078974982 &gt; N172Max=30，依照FS=2並給予最小體積應變vstr=0%</v>
+        <v>D50非數字，強制略過部份非液化條件檢核; D10非數字，強制略過部份非液化條件檢核; vibrationType非數字; Volumetric Strain(Tokimatsu And Seed): CSR大於0.6超過原研究範疇，強制改為0.6; Volumetric Strain(Tokimatsu And Seed): 出現外插情形 N160=37.150772494769974 &gt; N160Max=36.7，依照CSR=0.6並給予最小體積應變vstr=0.1%; Volumetric Strain(Ishihara And Yoshimine): 出現外插情形 N172=30.958977078974982 &gt; N172Max=30，依照FS=2並給予最小體積應變vstr=0%</v>
       </c>
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.3">
@@ -10579,7 +11037,7 @@
       </c>
       <c r="I80" s="1" t="str">
         <f>mat!EB5</f>
-        <v>D50 非數字，略過部份非液化條件檢核, D10 非數字，略過部份非液化條件檢核, vibrationType 非數字, vibrationType[0] 不等於 1 或 2，更改為預設值1, Volumetric Strain(Tokimatsu And Seed): CSR大於0.6超過原研究範疇，強制改為0.6, Volumetric Strain(Tokimatsu And Seed): 出現外插情形 N160=38.05808075175254 &gt; N160Max=36.7，依照CSR=0.6並給予最小體積應變vstr=0.1%, Volumetric Strain(Ishihara And Yoshimine): 出現外插情形 N172=31.715067293127117 &gt; N172Max=30，依照FS=2並給予最小體積應變vstr=0%</v>
+        <v>D50非數字，強制略過部份非液化條件檢核; D10非數字，強制略過部份非液化條件檢核; vibrationType非數字; Volumetric Strain(Tokimatsu And Seed): CSR大於0.6超過原研究範疇，強制改為0.6; Volumetric Strain(Tokimatsu And Seed): 出現外插情形 N160=38.05808075175254 &gt; N160Max=36.7，依照CSR=0.6並給予最小體積應變vstr=0.1%; Volumetric Strain(Ishihara And Yoshimine): 出現外插情形 N172=31.715067293127117 &gt; N172Max=30，依照FS=2並給予最小體積應變vstr=0%</v>
       </c>
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.3">
@@ -10617,7 +11075,7 @@
       </c>
       <c r="I81" s="1" t="str">
         <f>mat!EB6</f>
-        <v>D50 非數字，略過部份非液化條件檢核, D10 非數字，略過部份非液化條件檢核, vibrationType 非數字, vibrationType[0] 不等於 1 或 2，更改為預設值1</v>
+        <v>D50非數字，強制略過部份非液化條件檢核; D10非數字，強制略過部份非液化條件檢核; vibrationType非數字</v>
       </c>
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.3">
@@ -10655,7 +11113,7 @@
       </c>
       <c r="I82" s="1" t="str">
         <f>mat!EB7</f>
-        <v>D50 非數字，略過部份非液化條件檢核, D10 非數字，略過部份非液化條件檢核, vibrationType 非數字, vibrationType[0] 不等於 1 或 2，更改為預設值1</v>
+        <v>D50非數字，強制略過部份非液化條件檢核; D10非數字，強制略過部份非液化條件檢核; vibrationType非數字</v>
       </c>
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.3">
@@ -10693,7 +11151,7 @@
       </c>
       <c r="I83" s="1" t="str">
         <f>mat!EB8</f>
-        <v>D50 非數字，略過部份非液化條件檢核, D10 非數字，略過部份非液化條件檢核, PI 非數字與非NP，略過部份非液化條件檢核, vibrationType 非數字, vibrationType[0] 不等於 1 或 2，更改為預設值1</v>
+        <v>PI非數字與非NP，強制略過部份非液化條件檢核; D50非數字，強制略過部份非液化條件檢核; D10非數字，強制略過部份非液化條件檢核; vibrationType非數字</v>
       </c>
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.3">
@@ -10731,7 +11189,7 @@
       </c>
       <c r="I84" s="1" t="str">
         <f>mat!EB9</f>
-        <v>D50 非數字，略過部份非液化條件檢核, D10 非數字，略過部份非液化條件檢核, PI 非數字與非NP，略過部份非液化條件檢核, vibrationType 非數字, vibrationType[0] 不等於 1 或 2，更改為預設值1</v>
+        <v>PI非數字與非NP，強制略過部份非液化條件檢核; D50非數字，強制略過部份非液化條件檢核; D10非數字，強制略過部份非液化條件檢核; vibrationType非數字</v>
       </c>
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.3">
@@ -10769,7 +11227,7 @@
       </c>
       <c r="I85" s="1" t="str">
         <f>mat!EB10</f>
-        <v>D50 非數字，略過部份非液化條件檢核, D10 非數字，略過部份非液化條件檢核, PI 非數字與非NP，略過部份非液化條件檢核, vibrationType 非數字, vibrationType[0] 不等於 1 或 2，更改為預設值1</v>
+        <v>PI非數字與非NP，強制略過部份非液化條件檢核; D50非數字，強制略過部份非液化條件檢核; D10非數字，強制略過部份非液化條件檢核; vibrationType非數字</v>
       </c>
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.3">
@@ -10807,7 +11265,7 @@
       </c>
       <c r="I86" s="1" t="str">
         <f>mat!EB11</f>
-        <v>D50 非數字，略過部份非液化條件檢核, D10 非數字，略過部份非液化條件檢核, PI 非數字與非NP，略過部份非液化條件檢核, vibrationType 非數字, vibrationType[0] 不等於 1 或 2，更改為預設值1</v>
+        <v>PI非數字與非NP，強制略過部份非液化條件檢核; D50非數字，強制略過部份非液化條件檢核; D10非數字，強制略過部份非液化條件檢核; vibrationType非數字</v>
       </c>
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.3">
@@ -10845,7 +11303,7 @@
       </c>
       <c r="I87" s="1" t="str">
         <f>mat!EB12</f>
-        <v>D50 非數字，略過部份非液化條件檢核, D10 非數字，略過部份非液化條件檢核</v>
+        <v/>
       </c>
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.3">
@@ -10883,7 +11341,7 @@
       </c>
       <c r="I88" s="1" t="str">
         <f>mat!EB13</f>
-        <v>D50 非數字，略過部份非液化條件檢核, D10 非數字，略過部份非液化條件檢核</v>
+        <v/>
       </c>
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.3">
@@ -10921,7 +11379,7 @@
       </c>
       <c r="I89" s="1" t="str">
         <f>mat!EB14</f>
-        <v>D50 非數字，略過部份非液化條件檢核, D10 非數字，略過部份非液化條件檢核</v>
+        <v/>
       </c>
     </row>
     <row r="91" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
@@ -11073,7 +11531,7 @@
       </c>
       <c r="I94" s="1" t="str">
         <f>mat!EQ4</f>
-        <v>Volumetric Strain(Tokimatsu And Seed): 出現外插情形 N160=37.150772494769974 &gt; N160Max=33.348948148804865，依照CSR=0.3996625660206793並給予最小體積應變vstr=0.1%, Volumetric Strain(Ishihara And Yoshimine): 出現外插情形 N172=30.958977078974982 &gt; N172Max=30，依照FS=2並給予最小體積應變vstr=0%</v>
+        <v>Volumetric Strain(Tokimatsu And Seed): 出現外插情形 N160=37.150772494769974 &gt; N160Max=33.348948148804865，依照CSR=0.3996625660206793並給予最小體積應變vstr=0.1%; Volumetric Strain(Ishihara And Yoshimine): 出現外插情形 N172=30.958977078974982 &gt; N172Max=30，依照FS=2並給予最小體積應變vstr=0%</v>
       </c>
     </row>
     <row r="95" spans="1:9" x14ac:dyDescent="0.3">
@@ -11111,7 +11569,7 @@
       </c>
       <c r="I95" s="1" t="str">
         <f>mat!EQ5</f>
-        <v>Volumetric Strain(Tokimatsu And Seed): 出現外插情形 N160=38.05808075175254 &gt; N160Max=33.10466537238953，依照CSR=0.3919704067448309並給予最小體積應變vstr=0.1%, Volumetric Strain(Ishihara And Yoshimine): 出現外插情形 N172=31.715067293127117 &gt; N172Max=30，依照FS=2並給予最小體積應變vstr=0%</v>
+        <v>Volumetric Strain(Tokimatsu And Seed): 出現外插情形 N160=38.05808075175254 &gt; N160Max=33.10466537238953，依照CSR=0.3919704067448309並給予最小體積應變vstr=0.1%; Volumetric Strain(Ishihara And Yoshimine): 出現外插情形 N172=31.715067293127117 &gt; N172Max=30，依照FS=2並給予最小體積應變vstr=0%</v>
       </c>
     </row>
     <row r="96" spans="1:9" x14ac:dyDescent="0.3">

</xml_diff>